<commit_message>
LMDI: Fjernet address.extension[propertyInformation] fra pasient og organisasjon. Oppdaterte kort-beskrivelsen til Legemiddel.ingredient cc527da4d6f3ee25bff8427da14d523ecd168561
</commit_message>
<xml_diff>
--- a/currentbuild/StructureDefinition-lmdi-medication.xlsx
+++ b/currentbuild/StructureDefinition-lmdi-medication.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4637" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4637" uniqueCount="458">
   <si>
     <t>Property</t>
   </si>
@@ -1279,9 +1279,6 @@
   <si>
     <t xml:space="preserve">BackboneElement
 </t>
-  </si>
-  <si>
-    <t>Virkestoff(er) i legemiddelet</t>
   </si>
   <si>
     <t>Virkestoff(er) som inngår i legemiddelet. Skal fylles ut hvis code ikke har verdi. Bør fylles ut hvis code.coding[LokaltLegemiddel] har verdi.</t>
@@ -14678,10 +14675,10 @@
         <v>408</v>
       </c>
       <c r="M113" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="N113" t="s" s="2">
         <v>409</v>
-      </c>
-      <c r="N113" t="s" s="2">
-        <v>410</v>
       </c>
       <c r="O113" s="2"/>
       <c r="P113" t="s" s="2">
@@ -14749,7 +14746,7 @@
         <v>77</v>
       </c>
       <c r="AL113" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AM113" t="s" s="2">
         <v>77</v>
@@ -14760,10 +14757,10 @@
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B114" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" t="s" s="2">
@@ -14872,10 +14869,10 @@
     </row>
     <row r="115" hidden="true">
       <c r="A115" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B115" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C115" s="2"/>
       <c r="D115" t="s" s="2">
@@ -14986,14 +14983,14 @@
     </row>
     <row r="116" hidden="true">
       <c r="A116" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B116" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E116" s="2"/>
       <c r="F116" t="s" s="2">
@@ -15015,10 +15012,10 @@
         <v>132</v>
       </c>
       <c r="L116" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="M116" t="s" s="2">
         <v>416</v>
-      </c>
-      <c r="M116" t="s" s="2">
-        <v>417</v>
       </c>
       <c r="N116" t="s" s="2">
         <v>149</v>
@@ -15073,7 +15070,7 @@
         <v>77</v>
       </c>
       <c r="AF116" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AG116" t="s" s="2">
         <v>78</v>
@@ -15102,10 +15099,10 @@
     </row>
     <row r="117" hidden="true">
       <c r="A117" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B117" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" t="s" s="2">
@@ -15128,17 +15125,17 @@
         <v>77</v>
       </c>
       <c r="K117" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="L117" t="s" s="2">
         <v>420</v>
       </c>
-      <c r="L117" t="s" s="2">
+      <c r="M117" t="s" s="2">
         <v>421</v>
-      </c>
-      <c r="M117" t="s" s="2">
-        <v>422</v>
       </c>
       <c r="N117" s="2"/>
       <c r="O117" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="P117" t="s" s="2">
         <v>77</v>
@@ -15175,7 +15172,7 @@
         <v>77</v>
       </c>
       <c r="AB117" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="AC117" s="2"/>
       <c r="AD117" t="s" s="2">
@@ -15185,7 +15182,7 @@
         <v>136</v>
       </c>
       <c r="AF117" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AG117" t="s" s="2">
         <v>87</v>
@@ -15203,24 +15200,24 @@
         <v>166</v>
       </c>
       <c r="AL117" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="AM117" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN117" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="AM117" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN117" t="s" s="2">
-        <v>426</v>
       </c>
     </row>
     <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
+        <v>426</v>
+      </c>
+      <c r="B118" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="C118" t="s" s="2">
         <v>427</v>
-      </c>
-      <c r="B118" t="s" s="2">
-        <v>419</v>
-      </c>
-      <c r="C118" t="s" s="2">
-        <v>428</v>
       </c>
       <c r="D118" t="s" s="2">
         <v>77</v>
@@ -15242,17 +15239,17 @@
         <v>77</v>
       </c>
       <c r="K118" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="L118" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="M118" t="s" s="2">
         <v>421</v>
-      </c>
-      <c r="M118" t="s" s="2">
-        <v>422</v>
       </c>
       <c r="N118" s="2"/>
       <c r="O118" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="P118" t="s" s="2">
         <v>77</v>
@@ -15301,7 +15298,7 @@
         <v>77</v>
       </c>
       <c r="AF118" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AG118" t="s" s="2">
         <v>87</v>
@@ -15319,24 +15316,24 @@
         <v>166</v>
       </c>
       <c r="AL118" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="AM118" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN118" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="AM118" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN118" t="s" s="2">
-        <v>426</v>
       </c>
     </row>
     <row r="119" hidden="true">
       <c r="A119" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="B119" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="C119" t="s" s="2">
         <v>430</v>
-      </c>
-      <c r="B119" t="s" s="2">
-        <v>419</v>
-      </c>
-      <c r="C119" t="s" s="2">
-        <v>431</v>
       </c>
       <c r="D119" t="s" s="2">
         <v>77</v>
@@ -15361,14 +15358,14 @@
         <v>160</v>
       </c>
       <c r="L119" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="M119" t="s" s="2">
         <v>421</v>
-      </c>
-      <c r="M119" t="s" s="2">
-        <v>422</v>
       </c>
       <c r="N119" s="2"/>
       <c r="O119" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="P119" t="s" s="2">
         <v>77</v>
@@ -15415,7 +15412,7 @@
         <v>77</v>
       </c>
       <c r="AF119" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AG119" t="s" s="2">
         <v>87</v>
@@ -15433,21 +15430,21 @@
         <v>166</v>
       </c>
       <c r="AL119" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="AM119" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN119" t="s" s="2">
         <v>425</v>
-      </c>
-      <c r="AM119" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN119" t="s" s="2">
-        <v>426</v>
       </c>
     </row>
     <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B120" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" t="s" s="2">
@@ -15473,14 +15470,14 @@
         <v>236</v>
       </c>
       <c r="L120" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="M120" t="s" s="2">
         <v>433</v>
-      </c>
-      <c r="M120" t="s" s="2">
-        <v>434</v>
       </c>
       <c r="N120" s="2"/>
       <c r="O120" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="P120" t="s" s="2">
         <v>77</v>
@@ -15529,7 +15526,7 @@
         <v>77</v>
       </c>
       <c r="AF120" t="s" s="2">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="AG120" t="s" s="2">
         <v>78</v>
@@ -15547,7 +15544,7 @@
         <v>77</v>
       </c>
       <c r="AL120" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="AM120" t="s" s="2">
         <v>77</v>
@@ -15558,10 +15555,10 @@
     </row>
     <row r="121" hidden="true">
       <c r="A121" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B121" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C121" s="2"/>
       <c r="D121" t="s" s="2">
@@ -15587,10 +15584,10 @@
         <v>402</v>
       </c>
       <c r="L121" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="M121" t="s" s="2">
         <v>438</v>
-      </c>
-      <c r="M121" t="s" s="2">
-        <v>439</v>
       </c>
       <c r="N121" s="2"/>
       <c r="O121" s="2"/>
@@ -15641,7 +15638,7 @@
         <v>77</v>
       </c>
       <c r="AF121" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AG121" t="s" s="2">
         <v>78</v>
@@ -15656,7 +15653,7 @@
         <v>99</v>
       </c>
       <c r="AK121" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AL121" t="s" s="2">
         <v>405</v>
@@ -15665,15 +15662,15 @@
         <v>77</v>
       </c>
       <c r="AN121" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B122" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" t="s" s="2">
@@ -15699,10 +15696,10 @@
         <v>407</v>
       </c>
       <c r="L122" t="s" s="2">
+        <v>442</v>
+      </c>
+      <c r="M122" t="s" s="2">
         <v>443</v>
-      </c>
-      <c r="M122" t="s" s="2">
-        <v>444</v>
       </c>
       <c r="N122" s="2"/>
       <c r="O122" s="2"/>
@@ -15753,7 +15750,7 @@
         <v>77</v>
       </c>
       <c r="AF122" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="AG122" t="s" s="2">
         <v>78</v>
@@ -15771,7 +15768,7 @@
         <v>352</v>
       </c>
       <c r="AL122" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AM122" t="s" s="2">
         <v>77</v>
@@ -15782,10 +15779,10 @@
     </row>
     <row r="123" hidden="true">
       <c r="A123" t="s" s="2">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B123" t="s" s="2">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C123" s="2"/>
       <c r="D123" t="s" s="2">
@@ -15894,10 +15891,10 @@
     </row>
     <row r="124" hidden="true">
       <c r="A124" t="s" s="2">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B124" t="s" s="2">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C124" s="2"/>
       <c r="D124" t="s" s="2">
@@ -16008,14 +16005,14 @@
     </row>
     <row r="125" hidden="true">
       <c r="A125" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B125" t="s" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C125" s="2"/>
       <c r="D125" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E125" s="2"/>
       <c r="F125" t="s" s="2">
@@ -16037,10 +16034,10 @@
         <v>132</v>
       </c>
       <c r="L125" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="M125" t="s" s="2">
         <v>416</v>
-      </c>
-      <c r="M125" t="s" s="2">
-        <v>417</v>
       </c>
       <c r="N125" t="s" s="2">
         <v>149</v>
@@ -16095,7 +16092,7 @@
         <v>77</v>
       </c>
       <c r="AF125" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AG125" t="s" s="2">
         <v>78</v>
@@ -16124,10 +16121,10 @@
     </row>
     <row r="126" hidden="true">
       <c r="A126" t="s" s="2">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B126" t="s" s="2">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" t="s" s="2">
@@ -16153,10 +16150,10 @@
         <v>171</v>
       </c>
       <c r="L126" t="s" s="2">
+        <v>449</v>
+      </c>
+      <c r="M126" t="s" s="2">
         <v>450</v>
-      </c>
-      <c r="M126" t="s" s="2">
-        <v>451</v>
       </c>
       <c r="N126" s="2"/>
       <c r="O126" s="2"/>
@@ -16207,7 +16204,7 @@
         <v>77</v>
       </c>
       <c r="AF126" t="s" s="2">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="AG126" t="s" s="2">
         <v>78</v>
@@ -16231,15 +16228,15 @@
         <v>77</v>
       </c>
       <c r="AN126" t="s" s="2">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="127" hidden="true">
       <c r="A127" t="s" s="2">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B127" t="s" s="2">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C127" s="2"/>
       <c r="D127" t="s" s="2">
@@ -16262,13 +16259,13 @@
         <v>77</v>
       </c>
       <c r="K127" t="s" s="2">
+        <v>453</v>
+      </c>
+      <c r="L127" t="s" s="2">
         <v>454</v>
       </c>
-      <c r="L127" t="s" s="2">
+      <c r="M127" t="s" s="2">
         <v>455</v>
-      </c>
-      <c r="M127" t="s" s="2">
-        <v>456</v>
       </c>
       <c r="N127" s="2"/>
       <c r="O127" s="2"/>
@@ -16319,7 +16316,7 @@
         <v>77</v>
       </c>
       <c r="AF127" t="s" s="2">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="AG127" t="s" s="2">
         <v>78</v>
@@ -16337,13 +16334,13 @@
         <v>352</v>
       </c>
       <c r="AL127" t="s" s="2">
+        <v>456</v>
+      </c>
+      <c r="AM127" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AN127" t="s" s="2">
         <v>457</v>
-      </c>
-      <c r="AM127" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN127" t="s" s="2">
-        <v>458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>